<commit_message>
add file per node red
</commit_message>
<xml_diff>
--- a/interface agreement.xlsx
+++ b/interface agreement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\OneDrive\Desktop\Progetto_IoT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B2A889-54EA-4CD9-AB40-4D966EED54A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DCEBA1B-D92A-4407-B5CC-C50EC059C72D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="99">
   <si>
     <t xml:space="preserve">controlla che last up date sia minore di 120 secondi per eliminare i device che sono offline o non funzionanti il check deve essere fatto ogni 60 secondi </t>
   </si>
@@ -376,16 +376,53 @@
                 }
 }</t>
   </si>
+  <si>
+    <t>THING SPEAK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature </t>
+  </si>
+  <si>
+    <t>Actuator/Energy</t>
+  </si>
+  <si>
+    <t>Photon</t>
+  </si>
+  <si>
+    <t>prendere il grafico e calcolare la quantità di Energia attraverso dei calcoli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prendere il grafico e calcolare la quantità di Energia proveniente dai fotoni </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inserire i valori dei sensori nel grafico su thingspeak utilizzato una GET request </t>
+  </si>
+  <si>
+    <t>https://api.thingspeak.com/channels/2105394/fields/1.json?api_key=CUS2V05KYP2RIEAF&amp;results=2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://api.thingspeak.com/update?api_key=CUS2V05KYP2RIEAF&amp;field1=2 </t>
+  </si>
+  <si>
+    <t>https://it.mathworks.com/help/thingspeak/readfield.html;jsessionid=ae35524e858f69d777d4aa1a0827</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -552,7 +589,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -567,106 +604,128 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -884,19 +943,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1007"/>
+  <dimension ref="A1:F1009"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="C28" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28.88671875" customWidth="1"/>
     <col min="2" max="2" width="35" customWidth="1"/>
-    <col min="3" max="3" width="67.88671875" customWidth="1"/>
-    <col min="4" max="4" width="43.109375" customWidth="1"/>
-    <col min="5" max="5" width="61.33203125" customWidth="1"/>
+    <col min="3" max="3" width="75" customWidth="1"/>
+    <col min="4" max="4" width="90.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="89.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1291,7 +1350,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="12" t="s">
         <v>57</v>
       </c>
@@ -1302,7 +1361,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="2:5" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="12" t="s">
         <v>59</v>
       </c>
@@ -1313,7 +1372,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="26" t="s">
         <v>61</v>
       </c>
@@ -1324,7 +1383,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="26" t="s">
         <v>63</v>
       </c>
@@ -1338,7 +1397,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="26" t="s">
         <v>67</v>
       </c>
@@ -1352,17 +1411,60 @@
         <v>69</v>
       </c>
     </row>
-    <row r="38" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="39" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="40" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="41" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="46" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="47" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="48" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="39" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="39" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B42" s="39"/>
+    </row>
+    <row r="43" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B43" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="C43" s="39" t="s">
+        <v>95</v>
+      </c>
+      <c r="D43" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="E43" s="40"/>
+    </row>
+    <row r="44" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="39"/>
+      <c r="C44" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="D44" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="E44" s="28" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="C45" s="39" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C46" s="39" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="51" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2322,6 +2424,8 @@
     <row r="1005" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1006" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1007" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1008" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1009" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
@@ -2338,8 +2442,11 @@
     <hyperlink ref="C16" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
     <hyperlink ref="C17" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
     <hyperlink ref="C18" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="D44" r:id="rId15" xr:uid="{0BBE319F-290D-4FC3-B920-D7978EA7A414}"/>
+    <hyperlink ref="D43" r:id="rId16" xr:uid="{6E7C4539-EA81-4693-ABF7-2A9C1E71B7AD}"/>
+    <hyperlink ref="E44" r:id="rId17" xr:uid="{42B480F9-975A-49FD-91FD-51D227F19388}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId15"/>
+  <pageSetup orientation="landscape" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add the battery put method
</commit_message>
<xml_diff>
--- a/interface agreement.xlsx
+++ b/interface agreement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\an.geraci\Dropbox (Politecnico Di Torino Studenti)\Battery_Charger_Smart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B7D1765-7BCA-410A-8C2B-41FCA9D8CE29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD9ED67-6CA4-459D-849B-50E9A59B84B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="102">
   <si>
     <t xml:space="preserve">controlla che last up date sia minore di 120 secondi per eliminare i device che sono offline o non funzionanti il check deve essere fatto ogni 60 secondi </t>
   </si>
@@ -408,6 +408,15 @@
   </si>
   <si>
     <t>Add Agenda Date</t>
+  </si>
+  <si>
+    <t>Update the battery value</t>
+  </si>
+  <si>
+    <t>{
+            "UserID":"1",
+            "value":'12'
+}</t>
   </si>
 </sst>
 </file>
@@ -943,10 +952,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1010"/>
+  <dimension ref="A1:F1011"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="D16" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1175,112 +1184,114 @@
       <c r="F17" s="34"/>
     </row>
     <row r="18" spans="1:6" ht="48" x14ac:dyDescent="0.3">
-      <c r="A18" s="15"/>
-      <c r="B18" s="2" t="s">
-        <v>29</v>
+      <c r="B18" s="12" t="s">
+        <v>100</v>
       </c>
       <c r="C18" s="16" t="s">
         <v>30</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="E18" s="36" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="120.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="17"/>
+        <v>101</v>
+      </c>
+      <c r="F18" s="34"/>
+    </row>
+    <row r="19" spans="1:6" ht="48" x14ac:dyDescent="0.3">
+      <c r="A19" s="15"/>
       <c r="B19" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="41" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>30</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="35" t="s">
+      <c r="E19" s="36" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="120.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="17"/>
+      <c r="B20" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="35" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="31" t="s">
+      <c r="C21" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D21" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="33"/>
-    </row>
-    <row r="21" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
+      <c r="E21" s="33"/>
     </row>
     <row r="22" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="2"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+    </row>
+    <row r="23" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B23" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="31" t="s">
+      <c r="C23" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D23" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E22" s="18"/>
-    </row>
-    <row r="23" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="2"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="18"/>
       <c r="E23" s="18"/>
     </row>
     <row r="24" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>38</v>
-      </c>
+      <c r="A24" s="2"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="2"/>
       <c r="D24" s="18"/>
       <c r="E24" s="18"/>
     </row>
     <row r="25" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C25" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="A25" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="18"/>
       <c r="E25" s="18"/>
     </row>
     <row r="26" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C26" s="21" t="s">
-        <v>43</v>
+        <v>39</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>40</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>41</v>
@@ -1290,38 +1301,38 @@
     <row r="27" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C27" s="21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E27" s="22" t="s">
-        <v>47</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="E27" s="18"/>
     </row>
     <row r="28" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E28" s="18"/>
+        <v>46</v>
+      </c>
+      <c r="E28" s="22" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C29" s="20" t="s">
-        <v>51</v>
+        <v>48</v>
+      </c>
+      <c r="C29" s="21" t="s">
+        <v>49</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>41</v>
@@ -1331,10 +1342,10 @@
     <row r="30" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C30" s="23" t="s">
-        <v>53</v>
+        <v>50</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>51</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>41</v>
@@ -1342,56 +1353,58 @@
       <c r="E30" s="18"/>
     </row>
     <row r="31" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="E31" s="18"/>
     </row>
     <row r="32" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E32" s="18"/>
     </row>
-    <row r="33" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="32" t="s">
+    <row r="33" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E33" s="18"/>
+    </row>
+    <row r="34" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B34" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="E34" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="12" t="s">
+    <row r="35" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="D34" s="24" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="D35" s="24" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="C36" s="25" t="s">
-        <v>62</v>
+    <row r="36" spans="1:5" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="D36" s="24" t="s">
         <v>2</v>
@@ -1399,85 +1412,95 @@
     </row>
     <row r="37" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="25" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C37" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="D37" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="E37" s="25" t="s">
-        <v>66</v>
+        <v>62</v>
+      </c>
+      <c r="D37" s="24" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="25" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C38" s="25" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D38" s="26" t="s">
         <v>65</v>
       </c>
       <c r="E38" s="25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C39" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="D39" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="E39" s="25" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="40" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="41" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="38" t="s">
+    <row r="41" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="38" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="38" t="s">
+    <row r="43" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="38" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="38"/>
-    </row>
-    <row r="44" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="38" t="s">
+    <row r="44" spans="1:5" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B44" s="38"/>
+    </row>
+    <row r="45" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B45" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="C44" s="38" t="s">
+      <c r="C45" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="D44" s="40" t="s">
+      <c r="D45" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="E44" s="39"/>
-    </row>
-    <row r="45" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="38"/>
-      <c r="C45" s="38" t="s">
+      <c r="E45" s="39"/>
+    </row>
+    <row r="46" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="38"/>
+      <c r="C46" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="D45" s="27" t="s">
+      <c r="D46" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="E45" s="27" t="s">
+      <c r="E46" s="27" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="38" t="s">
+    <row r="47" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="C46" s="38" t="s">
+      <c r="C47" s="38" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C47" s="38" t="s">
+    <row r="48" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C48" s="38" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="51" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2440,6 +2463,7 @@
     <row r="1008" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1009" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1010" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1011" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
@@ -2452,15 +2476,16 @@
     <hyperlink ref="C12" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
     <hyperlink ref="C13" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
     <hyperlink ref="C14" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="C19" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="D45" r:id="rId12" xr:uid="{0BBE319F-290D-4FC3-B920-D7978EA7A414}"/>
-    <hyperlink ref="D44" r:id="rId13" xr:uid="{6E7C4539-EA81-4693-ABF7-2A9C1E71B7AD}"/>
-    <hyperlink ref="E45" r:id="rId14" xr:uid="{42B480F9-975A-49FD-91FD-51D227F19388}"/>
+    <hyperlink ref="C20" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="D46" r:id="rId12" xr:uid="{0BBE319F-290D-4FC3-B920-D7978EA7A414}"/>
+    <hyperlink ref="D45" r:id="rId13" xr:uid="{6E7C4539-EA81-4693-ABF7-2A9C1E71B7AD}"/>
+    <hyperlink ref="E46" r:id="rId14" xr:uid="{42B480F9-975A-49FD-91FD-51D227F19388}"/>
     <hyperlink ref="C16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
     <hyperlink ref="C17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="C18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="C19" r:id="rId17" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="C18" r:id="rId18" xr:uid="{65850376-DB59-4772-B4A7-DA0345366461}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId18"/>
+  <pageSetup orientation="landscape" r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
State Control added to the list of done things
</commit_message>
<xml_diff>
--- a/interface agreement.xlsx
+++ b/interface agreement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\an.geraci\Desktop\Battery_Charger_Smart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10522BC0-50E7-475F-B571-B0D970706E26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C8FEB4-0485-483C-8896-05470EAD745B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="121">
   <si>
     <t xml:space="preserve">controlla che last up date sia minore di 120 secondi per eliminare i device che sono offline o non funzionanti il check deve essere fatto ogni 60 secondi </t>
   </si>
@@ -476,7 +476,16 @@
     <t xml:space="preserve">battery percentage </t>
   </si>
   <si>
-    <t xml:space="preserve">TOPIC OF ALERT </t>
+    <t xml:space="preserve">TOPIC OF ALERT : Battery/IoT/project/UserID/1/statecontrol/AlertSMS </t>
+  </si>
+  <si>
+    <t>se funziona, se non funziona, se la macchina è a casa</t>
+  </si>
+  <si>
+    <t>se funziona, se non funziona, se è troppo bassa</t>
+  </si>
+  <si>
+    <t>se troppo alta, non può caricare</t>
   </si>
 </sst>
 </file>
@@ -1057,8 +1066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1014"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1662,15 +1671,33 @@
       <c r="B53" t="s">
         <v>113</v>
       </c>
+      <c r="C53" s="50" t="s">
+        <v>118</v>
+      </c>
+      <c r="D53" s="24" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="54" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>115</v>
       </c>
+      <c r="C54" s="50" t="s">
+        <v>120</v>
+      </c>
+      <c r="D54" s="24" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="55" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>116</v>
+      </c>
+      <c r="C55" s="50" t="s">
+        <v>119</v>
+      </c>
+      <c r="D55" s="24" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Add IP on the file
</commit_message>
<xml_diff>
--- a/interface agreement.xlsx
+++ b/interface agreement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\an.geraci\Desktop\Battery_Charger_Smart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EC1187E-2BB3-4F54-9D94-5E5D254E8F23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9BC5295-A6AD-4AAD-AEE0-F4AEF49F1FE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="134">
   <si>
     <t xml:space="preserve">controlla che last up date sia minore di 120 secondi per eliminare i device che sono offline o non funzionanti il check deve essere fatto ogni 60 secondi </t>
   </si>
@@ -502,16 +502,47 @@
   <si>
     <t>Battery/IoT/project/UserID/1/sensor/temperatureB</t>
   </si>
+  <si>
+    <t>"http://192.168.1.18:8080"</t>
+  </si>
+  <si>
+    <t>WiFi Anna</t>
+  </si>
+  <si>
+    <t>"http://172.17.0.1:8080"</t>
+  </si>
+  <si>
+    <t>Docker Container</t>
+  </si>
+  <si>
+    <t>"http://172.20.10.3:8080"</t>
+  </si>
+  <si>
+    <t>Iphone Anna hotspot</t>
+  </si>
+  <si>
+    <t>http://172.20.228.53:8080"</t>
+  </si>
+  <si>
+    <t>Ubuntu macchina Virtuale</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -656,6 +687,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -752,151 +789,155 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1115,8 +1156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1015"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1126,10 +1167,11 @@
     <col min="3" max="3" width="75" customWidth="1"/>
     <col min="4" max="4" width="90.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="89.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="26" width="8.6640625" customWidth="1"/>
+    <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
         <v>74</v>
       </c>
@@ -1146,7 +1188,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>67</v>
       </c>
@@ -1160,13 +1202,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="2"/>
       <c r="C3" s="5"/>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>68</v>
       </c>
@@ -1176,7 +1218,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>2</v>
       </c>
@@ -1193,7 +1235,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="10" t="s">
         <v>5</v>
       </c>
@@ -1203,8 +1245,14 @@
       <c r="D6" s="9" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E6" s="58" t="s">
+        <v>126</v>
+      </c>
+      <c r="F6" s="59" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="10" t="s">
         <v>7</v>
       </c>
@@ -1214,8 +1262,14 @@
       <c r="D7" s="9" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E7" s="58" t="s">
+        <v>128</v>
+      </c>
+      <c r="F7" s="59" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="10" t="s">
         <v>9</v>
       </c>
@@ -1225,8 +1279,14 @@
       <c r="D8" s="9" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E8" s="58" t="s">
+        <v>130</v>
+      </c>
+      <c r="F8" s="59" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>11</v>
       </c>
@@ -1236,8 +1296,14 @@
       <c r="D9" s="9" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E9" s="58" t="s">
+        <v>132</v>
+      </c>
+      <c r="F9" s="59" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="10" t="s">
         <v>12</v>
       </c>
@@ -1248,7 +1314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="10" t="s">
         <v>14</v>
       </c>
@@ -1259,7 +1325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="10" t="s">
         <v>16</v>
       </c>
@@ -1270,7 +1336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="396.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="396.6" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>18</v>
       </c>
@@ -1287,7 +1353,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="132" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="132" x14ac:dyDescent="0.3">
       <c r="B14" s="12" t="s">
         <v>22</v>
       </c>
@@ -1301,7 +1367,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="120.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="120.6" x14ac:dyDescent="0.3">
       <c r="B15" s="12" t="s">
         <v>96</v>
       </c>
@@ -1315,7 +1381,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="132.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
ADD some feature as for the agedaRemove method
</commit_message>
<xml_diff>
--- a/interface agreement.xlsx
+++ b/interface agreement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\an.geraci\Desktop\Battery_Charger_Smart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B62AC93-E2F5-4B08-B914-4854BE91E7DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A29EBA02-7CB2-4DA5-B4F7-E8D5E1669DEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="160">
   <si>
     <t xml:space="preserve">controlla che last up date sia minore di 120 secondi per eliminare i device che sono offline o non funzionanti il check deve essere fatto ogni 60 secondi </t>
   </si>
@@ -566,9 +566,6 @@
     <t>to see the impegni on Monday saved in the Agenda</t>
   </si>
   <si>
-    <t>/AgendaMondayChange</t>
-  </si>
-  <si>
     <t>done (POST request)</t>
   </si>
   <si>
@@ -578,22 +575,34 @@
     <t>/AgendaMondayRemove</t>
   </si>
   <si>
-    <t xml:space="preserve">To change </t>
-  </si>
-  <si>
     <t>To Remove</t>
   </si>
   <si>
     <t>Remove the Agenda date</t>
   </si>
   <si>
-    <t>http://127.0.0.1:8080/Agenda/Remove</t>
-  </si>
-  <si>
-    <t>http://127.0.0.1:8080/Agenda/Update</t>
-  </si>
-  <si>
-    <t>DELETE</t>
+    <t>http://127.0.0.1:8080/AgendaRemove</t>
+  </si>
+  <si>
+    <t>http://127.0.0.1:8080/AgendaUpdate</t>
+  </si>
+  <si>
+    <t>ONLY FROM POSTMAN</t>
+  </si>
+  <si>
+    <t>FROM ACTUATOR SENSOR TO UPDATE THE CATALOG</t>
+  </si>
+  <si>
+    <t>FROM BATTERY SENSOR TO UPDATE THE CATALOG</t>
+  </si>
+  <si>
+    <t>FROM SENSORS TO UPDATE THE CATALOG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FROM TELEGRAM BOT </t>
+  </si>
+  <si>
+    <t>FROM POSTMAN</t>
   </si>
 </sst>
 </file>
@@ -906,7 +915,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1055,9 +1064,6 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1076,6 +1082,15 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1293,10 +1308,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1019"/>
+  <dimension ref="A1:F1018"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1435,7 +1450,7 @@
       <c r="D9" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E9" s="62" t="s">
+      <c r="E9" s="61" t="s">
         <v>133</v>
       </c>
       <c r="F9" s="54" t="s">
@@ -1491,6 +1506,9 @@
       <c r="E13" s="14" t="s">
         <v>21</v>
       </c>
+      <c r="F13" s="70" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="14" spans="1:6" ht="132" x14ac:dyDescent="0.3">
       <c r="B14" s="12" t="s">
@@ -1505,6 +1523,9 @@
       <c r="E14" s="37" t="s">
         <v>24</v>
       </c>
+      <c r="F14" s="70" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="15" spans="1:6" ht="120.6" x14ac:dyDescent="0.3">
       <c r="B15" s="12" t="s">
@@ -1519,6 +1540,9 @@
       <c r="E15" s="35" t="s">
         <v>85</v>
       </c>
+      <c r="F15" s="70" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="132.6" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
@@ -1536,6 +1560,9 @@
       <c r="E16" s="34" t="s">
         <v>82</v>
       </c>
+      <c r="F16" s="70" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="48.6" x14ac:dyDescent="0.3">
       <c r="B17" s="12" t="s">
@@ -1550,7 +1577,9 @@
       <c r="E17" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="F17" s="34"/>
+      <c r="F17" s="71" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="18" spans="1:6" ht="48" x14ac:dyDescent="0.3">
       <c r="B18" s="12" t="s">
@@ -1565,7 +1594,9 @@
       <c r="E18" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="F18" s="34"/>
+      <c r="F18" s="71" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="19" spans="1:6" ht="48" x14ac:dyDescent="0.3">
       <c r="A19" s="15"/>
@@ -1581,6 +1612,9 @@
       <c r="E19" s="36" t="s">
         <v>84</v>
       </c>
+      <c r="F19" s="71" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="20" spans="1:6" ht="120.6" x14ac:dyDescent="0.3">
       <c r="A20" s="17"/>
@@ -1588,7 +1622,7 @@
         <v>31</v>
       </c>
       <c r="C20" s="39" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>30</v>
@@ -1596,22 +1630,26 @@
       <c r="E20" s="35" t="s">
         <v>85</v>
       </c>
+      <c r="F20" s="70" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="21" spans="1:6" ht="120.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
-        <v>156</v>
-      </c>
+      <c r="A21" s="69"/>
       <c r="B21" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C21" s="39" t="s">
-        <v>154</v>
-      </c>
-      <c r="D21" s="67" t="s">
-        <v>62</v>
+        <v>152</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="E21" s="35" t="s">
         <v>85</v>
+      </c>
+      <c r="F21" s="70" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1847,176 +1885,176 @@
         <v>57</v>
       </c>
       <c r="D41" s="24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="C42" s="67" t="s">
         <v>150</v>
       </c>
-      <c r="C42" s="68" t="s">
-        <v>152</v>
-      </c>
-      <c r="D42" s="69" t="s">
-        <v>149</v>
+      <c r="D42" s="68" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="C43" s="68" t="s">
-        <v>151</v>
-      </c>
-      <c r="D43" s="69" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C43" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="D44" s="67" t="s">
+      <c r="D43" s="66" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C44" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="D44" s="24" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="25" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C45" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="D45" s="24" t="s">
-        <v>1</v>
+        <v>61</v>
+      </c>
+      <c r="D45" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="E45" s="25" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="25" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C46" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="D46" s="26" t="s">
-        <v>62</v>
+        <v>65</v>
+      </c>
+      <c r="D46" s="24" t="s">
+        <v>1</v>
       </c>
       <c r="E46" s="25" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="C47" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="D47" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="E47" s="25" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="C48" s="50" t="s">
+        <v>109</v>
+      </c>
+    </row>
     <row r="49" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="32" t="s">
-        <v>108</v>
-      </c>
-      <c r="C49" s="50" t="s">
-        <v>109</v>
-      </c>
+      <c r="A49" s="58" t="s">
+        <v>86</v>
+      </c>
+      <c r="B49" s="59"/>
+      <c r="C49" s="59"/>
+      <c r="D49" s="55"/>
     </row>
     <row r="50" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="58" t="s">
-        <v>86</v>
-      </c>
-      <c r="B50" s="59"/>
+      <c r="A50" s="59"/>
+      <c r="B50" s="58" t="s">
+        <v>87</v>
+      </c>
       <c r="C50" s="59"/>
       <c r="D50" s="55"/>
     </row>
-    <row r="51" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="59"/>
-      <c r="B51" s="58" t="s">
-        <v>87</v>
-      </c>
+      <c r="B51" s="58"/>
       <c r="C51" s="59"/>
       <c r="D51" s="55"/>
     </row>
-    <row r="52" spans="1:5" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="59"/>
-      <c r="B52" s="58"/>
-      <c r="C52" s="59"/>
-      <c r="D52" s="55"/>
-    </row>
-    <row r="53" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B52" s="58" t="s">
+        <v>88</v>
+      </c>
+      <c r="C52" s="58" t="s">
+        <v>92</v>
+      </c>
+      <c r="D52" s="56" t="s">
+        <v>94</v>
+      </c>
+      <c r="E52" s="38"/>
+    </row>
+    <row r="53" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="59"/>
-      <c r="B53" s="58" t="s">
-        <v>88</v>
-      </c>
+      <c r="B53" s="58"/>
       <c r="C53" s="58" t="s">
-        <v>92</v>
-      </c>
-      <c r="D53" s="56" t="s">
-        <v>94</v>
-      </c>
-      <c r="E53" s="38"/>
+        <v>90</v>
+      </c>
+      <c r="D53" s="57" t="s">
+        <v>93</v>
+      </c>
+      <c r="E53" s="27" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="54" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="59"/>
-      <c r="B54" s="58"/>
+      <c r="B54" s="58" t="s">
+        <v>89</v>
+      </c>
       <c r="C54" s="58" t="s">
-        <v>90</v>
-      </c>
-      <c r="D54" s="57" t="s">
-        <v>93</v>
-      </c>
-      <c r="E54" s="27" t="s">
-        <v>95</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="D54" s="55"/>
     </row>
     <row r="55" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="59"/>
-      <c r="B55" s="58" t="s">
-        <v>89</v>
-      </c>
+      <c r="A55" s="60"/>
+      <c r="B55" s="59"/>
       <c r="C55" s="58" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D55" s="55"/>
     </row>
-    <row r="56" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="60"/>
-      <c r="B56" s="59"/>
-      <c r="C56" s="58" t="s">
-        <v>91</v>
-      </c>
-      <c r="D56" s="55"/>
-    </row>
-    <row r="57" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A57" s="32" t="s">
+    <row r="56" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A56" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="B57" s="47" t="s">
+      <c r="B56" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="C57" s="49" t="s">
+      <c r="C56" s="49" t="s">
         <v>116</v>
       </c>
-      <c r="D57" s="51" t="s">
+      <c r="D56" s="51" t="s">
         <v>112</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="52" t="s">
+        <v>121</v>
+      </c>
+      <c r="C57" s="48" t="s">
+        <v>113</v>
+      </c>
+      <c r="D57" s="24" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B58" s="52" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C58" s="48" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D58" s="24" t="s">
         <v>1</v>
@@ -2024,79 +2062,69 @@
     </row>
     <row r="59" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B59" s="52" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C59" s="48" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D59" s="24" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="52" t="s">
-        <v>123</v>
-      </c>
-      <c r="C60" s="48" t="s">
-        <v>114</v>
-      </c>
-      <c r="D60" s="24" t="s">
-        <v>1</v>
-      </c>
-    </row>
+    <row r="60" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="61" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="62" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="63" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="64" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="63" t="s">
+    <row r="63" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="62" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="65" spans="2:3" ht="92.4" x14ac:dyDescent="0.3">
-      <c r="B65" s="66" t="s">
+    <row r="64" spans="1:5" ht="92.4" x14ac:dyDescent="0.3">
+      <c r="B64" s="65" t="s">
         <v>135</v>
       </c>
-      <c r="C65" s="64" t="s">
+      <c r="C64" s="63" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="66" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B66" s="65" t="s">
+    <row r="65" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B65" s="64" t="s">
         <v>136</v>
       </c>
-      <c r="C66" s="47" t="s">
+      <c r="C65" s="47" t="s">
         <v>142</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C66" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="67" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C67" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="68" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C68" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="69" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C69" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="70" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C70" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="71" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="72" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B72" t="s">
+    <row r="70" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="71" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B71" t="s">
         <v>143</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C71" t="s">
         <v>144</v>
       </c>
     </row>
+    <row r="72" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="73" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="74" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="75" spans="2:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3043,7 +3071,6 @@
     <row r="1016" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1017" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1018" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1019" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
@@ -3057,9 +3084,9 @@
     <hyperlink ref="C13" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
     <hyperlink ref="C14" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
     <hyperlink ref="C20" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="D54" r:id="rId12" xr:uid="{0BBE319F-290D-4FC3-B920-D7978EA7A414}"/>
-    <hyperlink ref="D53" r:id="rId13" xr:uid="{6E7C4539-EA81-4693-ABF7-2A9C1E71B7AD}"/>
-    <hyperlink ref="E54" r:id="rId14" xr:uid="{42B480F9-975A-49FD-91FD-51D227F19388}"/>
+    <hyperlink ref="D53" r:id="rId12" xr:uid="{0BBE319F-290D-4FC3-B920-D7978EA7A414}"/>
+    <hyperlink ref="D52" r:id="rId13" xr:uid="{6E7C4539-EA81-4693-ABF7-2A9C1E71B7AD}"/>
+    <hyperlink ref="E53" r:id="rId14" xr:uid="{42B480F9-975A-49FD-91FD-51D227F19388}"/>
     <hyperlink ref="C16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
     <hyperlink ref="C17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
     <hyperlink ref="C19" r:id="rId17" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>

</xml_diff>